<commit_message>
updated 2 languages + fix doi
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="214" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="256" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="650">
   <si>
     <t>Language</t>
   </si>
@@ -254,7 +254,7 @@
     <t>Sultanate of Brunei Darussalam</t>
   </si>
   <si>
-    <t> Limbang, Sarawak, Malaysia</t>
+    <t>Limbang, Sarawak, Malaysia</t>
   </si>
   <si>
     <t>Labuan, Labuan Federal Territory Malaysia</t>
@@ -263,7 +263,7 @@
     <t>Beaufort, Sabah, Malaysia</t>
   </si>
   <si>
-    <t> Miri, Sarawak, Malaysia</t>
+    <t>Miri, Sarawak, Malaysia</t>
   </si>
   <si>
     <t>http://dx.doi.org/10.1017/S0025100316000189</t>
@@ -698,7 +698,7 @@
     <t>Komotini,Thrace, Greece</t>
   </si>
   <si>
-    <t>Drosero, Xanthi, Thrace, Greece.</t>
+    <t>Drosero, Xanthi, Thrace, 671 00 Greece.</t>
   </si>
   <si>
     <t>http://dx.doi.org/10.1017/S0025100313000376</t>
@@ -1019,7 +1019,7 @@
     <t>Kumzari</t>
   </si>
   <si>
-    <t>Musandam Peninsula, Oman and Iran</t>
+    <t>Musandam Peninsula, Oman</t>
   </si>
   <si>
     <t>http://dx.doi.org/10.1017/S0025100311000314</t>
@@ -1163,7 +1163,7 @@
     <t>Neuquén, Argentina</t>
   </si>
   <si>
-    <t> La Pampa, Argentina</t>
+    <t>La Pampa, Argentina</t>
   </si>
   <si>
     <t>Río Negro, Argentina</t>
@@ -1361,6 +1361,9 @@
     <t>Ayers Rock, Australia</t>
   </si>
   <si>
+    <t>https://doi.org/10.1017/S0025100314000073</t>
+  </si>
+  <si>
     <t>https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Pitjantjatjara.zip</t>
   </si>
   <si>
@@ -1427,7 +1430,7 @@
     <t>Setswana (South African)</t>
   </si>
   <si>
-    <t>Taung, South Africa </t>
+    <t>Taung, South Africa</t>
   </si>
   <si>
     <t>http://dx.doi.org/10.1017/S0025100316000050</t>
@@ -1532,7 +1535,7 @@
     <t>Southeastern Pashayi</t>
   </si>
   <si>
-    <t>Dara-i-Nur, Nangarhar, Afghanistan </t>
+    <t>Kuz Kunar, Nangarhar, Afghanistan </t>
   </si>
   <si>
     <t>http://dx.doi.org/10.1017/S0025100313000133</t>
@@ -1941,6 +1944,27 @@
   </si>
   <si>
     <t>https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Upper-Sorbian.zip</t>
+  </si>
+  <si>
+    <t>Niuean</t>
+  </si>
+  <si>
+    <t>Niue</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1017/S0025100317000500</t>
+  </si>
+  <si>
+    <t>Hawaiian</t>
+  </si>
+  <si>
+    <t>Hawaii, USA</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1017/S0025100316000438</t>
+  </si>
+  <si>
+    <t>https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Hawaiian.zip</t>
   </si>
 </sst>
 </file>
@@ -1950,11 +1974,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1970,6 +1995,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2014,8 +2046,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2036,10 +2072,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J157"/>
+  <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B79" activeCellId="0" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3929,161 +3965,161 @@
       <c r="B107" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="G107" s="0" t="s">
-        <v>370</v>
+      <c r="G107" s="1" t="s">
+        <v>448</v>
       </c>
       <c r="H107" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I107" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="H108" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I108" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="H109" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I109" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="H110" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I110" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="H111" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I111" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="G112" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="H112" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I112" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G113" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="H113" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I113" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="G114" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="H114" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I114" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="G115" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="H115" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I115" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="G116" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="H116" s="0" t="s">
         <v>19</v>
@@ -4091,183 +4127,183 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="G117" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="H117" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I117" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="G118" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="H118" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I118" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="G119" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="H119" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I119" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G120" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="H120" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I120" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="G121" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H121" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I121" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="G122" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="H122" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I122" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="G123" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="H123" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I123" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="G124" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="H124" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I124" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="G125" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="H125" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I125" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="G126" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="H126" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I126" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="G127" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="H127" s="0" t="s">
         <v>19</v>
@@ -4278,30 +4314,30 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="G128" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="H128" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I128" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="G129" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="H129" s="0" t="s">
         <v>19</v>
@@ -4309,47 +4345,47 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="G130" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="H130" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I130" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="G131" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="H131" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I131" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="G132" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H132" s="0" t="s">
         <v>13</v>
@@ -4357,189 +4393,189 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="G133" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="H133" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I133" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="G134" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="H134" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I134" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="G135" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="H135" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I135" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="G136" s="0" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="H136" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I136" s="0" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C137" s="0" t="s">
         <v>139</v>
       </c>
       <c r="G137" s="0" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="H137" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I137" s="0" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="G138" s="0" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H138" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I138" s="0" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="G139" s="0" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="H139" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I139" s="0" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="G140" s="0" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="H140" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I140" s="0" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="G141" s="0" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="H141" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I141" s="0" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="G142" s="0" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="H142" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I142" s="0" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="G143" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="H143" s="0" t="s">
         <v>13</v>
@@ -4547,166 +4583,166 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="G144" s="0" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="H144" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I144" s="0" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="G145" s="0" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="H145" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I145" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="G146" s="0" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="H146" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I146" s="0" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="G147" s="0" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="H147" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I147" s="0" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="G148" s="0" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="H148" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I148" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="G149" s="0" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="H149" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I149" s="0" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="G150" s="0" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="H150" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I150" s="0" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="G151" s="0" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="H151" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I151" s="0" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="G152" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="H152" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I152" s="0" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="G153" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="H153" s="0" t="s">
         <v>19</v>
@@ -4717,73 +4753,107 @@
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="G154" s="0" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="H154" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I154" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="G155" s="0" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="H155" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I155" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="G156" s="0" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="H156" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I156" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="G157" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H157" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I157" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>643</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>644</v>
+      </c>
+      <c r="G158" s="0" t="s">
+        <v>645</v>
+      </c>
+      <c r="H158" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>646</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>647</v>
+      </c>
+      <c r="G159" s="0" t="s">
+        <v>648</v>
+      </c>
+      <c r="H159" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I159" s="0" t="s">
+        <v>649</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G107" r:id="rId1" display="https://doi.org/10.1017/S0025100314000073"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
update Nov 2018 - Central Lisu, Philippine English, Zwara (Zuwārah) Berber
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="662">
   <si>
     <t>Language</t>
   </si>
@@ -1968,6 +1968,39 @@
   </si>
   <si>
     <t>https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Hawaiian.zip</t>
+  </si>
+  <si>
+    <t>Central Lisu</t>
+  </si>
+  <si>
+    <t>ShiBaCha, Yingjiang, Dehong, Yunnan, China</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1017/S0025100318000129</t>
+  </si>
+  <si>
+    <t>Philippine English</t>
+  </si>
+  <si>
+    <t>Manila, Philippines</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1017/S0025100317000548</t>
+  </si>
+  <si>
+    <t>https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/PhilippineEnglish.zip</t>
+  </si>
+  <si>
+    <t>Zwara (Zuwārah) Berber</t>
+  </si>
+  <si>
+    <t>Zwara, Libya</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1017/S0025100317000135</t>
+  </si>
+  <si>
+    <t>https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Zwara-Berber.zip</t>
   </si>
 </sst>
 </file>
@@ -2064,10 +2097,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J159"/>
+  <dimension ref="A1:J162"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G107" activeCellId="0" sqref="G2:G151"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B160" activeCellId="0" sqref="B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4848,6 +4881,54 @@
         <v>650</v>
       </c>
     </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>651</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="G160" s="0" t="s">
+        <v>653</v>
+      </c>
+      <c r="H160" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>654</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>655</v>
+      </c>
+      <c r="G161" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="H161" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I161" s="0" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>658</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>659</v>
+      </c>
+      <c r="G162" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="H162" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I162" s="0" t="s">
+        <v>661</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
updated links to recordings + Bajau
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="753">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -2137,6 +2137,9 @@
     <t xml:space="preserve">https://doi.org/10.1017/S0025100318000336</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Hmu.zip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Seenku</t>
   </si>
   <si>
@@ -2146,6 +2149,9 @@
     <t xml:space="preserve">https://doi.org/10.1017/S0025100318000312</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Seenku.zip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cagliari Sardinian</t>
   </si>
   <si>
@@ -2203,6 +2209,9 @@
     <t xml:space="preserve">https://doi.org/10.1017/S0025100319000082</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/A'ingae.zip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Central Malagasy</t>
   </si>
   <si>
@@ -2212,6 +2221,9 @@
     <t xml:space="preserve">https://doi.org/10.1017/S0025100319000100</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Central-Malagasy.zip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Xiangxiang dialect of Chinese</t>
   </si>
   <si>
@@ -2221,6 +2233,9 @@
     <t xml:space="preserve">https://doi-org/10.1017/S002510031800035X</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Xiangxiang.zip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Scottish Gaelic</t>
   </si>
   <si>
@@ -2252,6 +2267,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://doi.org/10.1017/S0025100319000203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Khuzestani-Arabic.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indonesian Bajau (East Lombok)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100319000239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Indonesian-Bajau.zip</t>
   </si>
 </sst>
 </file>
@@ -2333,13 +2360,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -2423,24 +2454,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J186"/>
+  <dimension ref="A1:J187"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A147" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B171" activeCellId="0" sqref="B171"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B187" activeCellId="0" sqref="B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="87.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="38.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="102.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="175.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="175.27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -5470,178 +5501,212 @@
       <c r="H175" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="I175" s="2" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H176" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I176" s="1"/>
+      <c r="I176" s="2" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="H177" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="H178" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I178" s="1" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="H179" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I179" s="1" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="H180" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I180" s="1" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="H181" s="0" t="s">
         <v>19</v>
+      </c>
+      <c r="I181" s="0" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="H182" s="0" t="s">
         <v>19</v>
+      </c>
+      <c r="I182" s="0" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>731</v>
+        <v>734</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>735</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c r="H183" s="0" t="s">
         <v>19</v>
+      </c>
+      <c r="I183" s="0" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>733</v>
+        <v>738</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>734</v>
+        <v>739</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>735</v>
+        <v>740</v>
       </c>
       <c r="H184" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I184" s="1" t="s">
-        <v>736</v>
+        <v>741</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>738</v>
+        <v>743</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>739</v>
+        <v>744</v>
       </c>
       <c r="H185" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>740</v>
+        <v>745</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>742</v>
+        <v>747</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
       <c r="H186" s="0" t="s">
         <v>19</v>
+      </c>
+      <c r="I186" s="0" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="G187" s="0" t="s">
+        <v>751</v>
+      </c>
+      <c r="H187" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I187" s="0" t="s">
+        <v>752</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed typos in doi for Malacca Portuguese creole and Xiangxiang
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -2182,7 +2182,25 @@
     <t xml:space="preserve">Malacca, Malaysia</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/0.1017/S0025100319000033</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://doi.org/10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.1017/S0025100319000033</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Malacca-Portuguese.zip</t>
@@ -2230,7 +2248,25 @@
     <t xml:space="preserve">Xiangxiang, Hunan province, China</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi-org/10.1017/S002510031800035X</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://doi.org</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/10.1017/S002510031800035X</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Xiangxiang.zip</t>
@@ -2288,7 +2324,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2309,6 +2345,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2360,7 +2403,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2374,6 +2417,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2456,14 +2503,14 @@
   </sheetPr>
   <dimension ref="A1:J187"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B187" activeCellId="0" sqref="B187"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B163" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G183" activeCellId="0" sqref="G183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="87.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.94"/>
@@ -2471,7 +2518,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="38.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="102.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="175.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="175.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -5563,7 +5610,7 @@
       <c r="B179" s="0" t="s">
         <v>719</v>
       </c>
-      <c r="G179" s="1" t="s">
+      <c r="G179" s="3" t="s">
         <v>720</v>
       </c>
       <c r="H179" s="0" t="s">
@@ -5628,10 +5675,10 @@
       <c r="A183" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="B183" s="3" t="s">
+      <c r="B183" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="G183" s="1" t="s">
+      <c r="G183" s="3" t="s">
         <v>736</v>
       </c>
       <c r="H183" s="0" t="s">
@@ -5710,6 +5757,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G179" r:id="rId1" display="https://doi.org/10"/>
+    <hyperlink ref="G183" r:id="rId2" display="https://doi.org"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Eastern Andalusian Spanish and Saraiki Sokar
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="789">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -2363,6 +2363,30 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Zhushan-Mandarin.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Andalusian Spanish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almería, Andalusia, Spain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Eastern-Andalusian-Spanish.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saraiki Sokar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dera Ghazi Khan, Punjab, Pakistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/saraiki.zip</t>
   </si>
 </sst>
 </file>
@@ -2549,10 +2573,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J194"/>
+  <dimension ref="A1:J196"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A194" activeCellId="0" sqref="A194"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F172" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F196" activeCellId="0" sqref="F196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5923,6 +5947,40 @@
         <v>780</v>
       </c>
     </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="G195" s="0" t="s">
+        <v>783</v>
+      </c>
+      <c r="H195" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I195" s="0" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="G196" s="0" t="s">
+        <v>787</v>
+      </c>
+      <c r="H196" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I196" s="0" t="s">
+        <v>788</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
recording file name change + Khongso
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="793">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -2290,7 +2290,7 @@
     <t xml:space="preserve">https://doi.org/10.1017/S0025100319000264</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/kejom.zip</t>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kejom.zip</t>
   </si>
   <si>
     <t xml:space="preserve">Kazakh</t>
@@ -2302,7 +2302,7 @@
     <t xml:space="preserve">https://doi.org/10.1017/S0025100319000185</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/kazakh.zip</t>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kazakh.zip</t>
   </si>
   <si>
     <t xml:space="preserve">Jianchuan Bai</t>
@@ -2314,7 +2314,25 @@
     <t xml:space="preserve">https://doi.org/10.1017/S0025100319000379 </t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/jianchuan-bai.zip</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Jianchuan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-bai.ziB</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Kalasha (Bumburet variety) </t>
@@ -2326,7 +2344,25 @@
     <t xml:space="preserve">https://doi.org/10.1017/S0025100319000367</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/kalasha.zip</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kalasha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.zip</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Belarusian</t>
@@ -2338,7 +2374,25 @@
     <t xml:space="preserve">https://doi.org/10.1017/S0025100319000288 </t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/belarusian.zip</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Belarusian</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.zip</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Lili Wu Chinese</t>
@@ -2386,7 +2440,37 @@
     <t xml:space="preserve">https://doi.org/10.1017/S0025100320000328</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/saraiki.zip</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Saraiki</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.zip</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Khongso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paletwa Township, Southern Chin State, Myanmar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Khongso.zip</t>
   </si>
 </sst>
 </file>
@@ -2396,7 +2480,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2428,6 +2512,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -2475,7 +2566,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2493,6 +2584,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2573,10 +2672,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J196"/>
+  <dimension ref="A1:J197"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F172" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F196" activeCellId="0" sqref="F196"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E182" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I190" activeCellId="0" sqref="I190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5858,7 +5957,7 @@
       <c r="H189" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I189" s="2" t="s">
+      <c r="I189" s="5" t="s">
         <v>760</v>
       </c>
     </row>
@@ -5875,7 +5974,7 @@
       <c r="H190" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I190" s="0" t="s">
+      <c r="I190" s="6" t="s">
         <v>764</v>
       </c>
     </row>
@@ -5892,7 +5991,7 @@
       <c r="H191" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I191" s="0" t="s">
+      <c r="I191" s="6" t="s">
         <v>768</v>
       </c>
     </row>
@@ -5909,7 +6008,7 @@
       <c r="H192" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I192" s="0" t="s">
+      <c r="I192" s="6" t="s">
         <v>772</v>
       </c>
     </row>
@@ -5977,11 +6076,36 @@
       <c r="H196" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I196" s="0" t="s">
+      <c r="I196" s="6" t="s">
         <v>788</v>
       </c>
     </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="G197" s="0" t="s">
+        <v>791</v>
+      </c>
+      <c r="H197" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I197" s="0" t="s">
+        <v>792</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I188" r:id="rId1" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kejom"/>
+    <hyperlink ref="I189" r:id="rId2" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kazakh"/>
+    <hyperlink ref="I190" r:id="rId3" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Jianchuan"/>
+    <hyperlink ref="I191" r:id="rId4" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kalasha"/>
+    <hyperlink ref="I192" r:id="rId5" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Belarusian"/>
+    <hyperlink ref="I196" r:id="rId6" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Saraiki"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Trapezountian Pontic Greek, Dàgáárè, Ambel, Arabic dialect of Gaza City
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="809">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -2312,6 +2312,99 @@
   </si>
   <si>
     <t xml:space="preserve">https://doi.org/10.1017/S0025100319000379 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Jianchuan-bai.ziB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalasha (Bumburet variety) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chitral district, Khyber Pakhtunkwa Province, Pakistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100319000367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kalasha.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belarusian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minsk, Belarus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100319000288 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Belarusian.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lili Wu Chinese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lili, Wujiang district, Suzhou city, Jiangsu province, China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Lili-Wu-Chinese.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zhushan Mandarin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zhushan county, Shiyan city, Hubei province,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Zhushan-Mandarin.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Andalusian Spanish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almería, Andalusia, Spain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Eastern-Andalusian-Spanish.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saraiki Sokar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dera Ghazi Khan, Punjab, Pakistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Saraiki.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khongso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paletwa Township, Southern Chin State, Myanmar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Khongso.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trapezountian Pontic Greek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etoloakarnania, Greece </t>
   </si>
   <si>
     <r>
@@ -2322,7 +2415,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Jianchuan</t>
+      <t xml:space="preserve">https://doi.org/10.1017/S0025100320000201</t>
     </r>
     <r>
       <rPr>
@@ -2331,17 +2424,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">-bai.ziB</t>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Kalasha (Bumburet variety) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chitral district, Khyber Pakhtunkwa Province, Pakistan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1017/S0025100319000367</t>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Trapezountian-Greek.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dàgáárè (Central)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sombo, Nadowli-Kaleo district, Ghana </t>
   </si>
   <si>
     <r>
@@ -2352,7 +2445,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kalasha</t>
+      <t xml:space="preserve">https://doi.org/10.1017/S0025100320000225</t>
     </r>
     <r>
       <rPr>
@@ -2361,17 +2454,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">.zip</t>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Belarusian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minsk, Belarus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1017/S0025100319000288 </t>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Dagaare.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waigeo Island, Raja Ampat Regency, West Papua, Indonesia</t>
   </si>
   <si>
     <r>
@@ -2382,7 +2475,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Belarusian</t>
+      <t xml:space="preserve">https://doi.org/10.1017/S0025100320000237</t>
     </r>
     <r>
       <rPr>
@@ -2391,86 +2484,23 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">.zip</t>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Lili Wu Chinese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lili, Wujiang district, Suzhou city, Jiangsu province, China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000092</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Lili-Wu-Chinese.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zhushan Mandarin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zhushan county, Shiyan city, Hubei province,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Zhushan-Mandarin.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Andalusian Spanish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Almería, Andalusia, Spain </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Eastern-Andalusian-Spanish.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saraiki Sokar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dera Ghazi Khan, Punjab, Pakistan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000328</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Saraiki</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.zip</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Khongso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paletwa Township, Southern Chin State, Myanmar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000286</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Khongso.zip</t>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Ambel.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arabic dialect of Gaza City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaza City, Israel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Arabic-Dialect-Of-Gaza-City.zip</t>
   </si>
 </sst>
 </file>
@@ -2566,7 +2596,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2593,6 +2623,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2672,10 +2706,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J197"/>
+  <dimension ref="A1:J201"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E182" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I190" activeCellId="0" sqref="I190"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A149" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B201" activeCellId="0" sqref="B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6097,14 +6131,90 @@
         <v>792</v>
       </c>
     </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="G198" s="7" t="s">
+        <v>795</v>
+      </c>
+      <c r="H198" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I198" s="7" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="G199" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="H199" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I199" s="7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="G200" s="7" t="s">
+        <v>803</v>
+      </c>
+      <c r="H200" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I200" s="7" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="G201" s="7" t="s">
+        <v>807</v>
+      </c>
+      <c r="H201" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I201" s="7" t="s">
+        <v>808</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I188" r:id="rId1" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kejom"/>
-    <hyperlink ref="I189" r:id="rId2" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kazakh"/>
-    <hyperlink ref="I190" r:id="rId3" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Jianchuan"/>
-    <hyperlink ref="I191" r:id="rId4" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kalasha"/>
-    <hyperlink ref="I192" r:id="rId5" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Belarusian"/>
-    <hyperlink ref="I196" r:id="rId6" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Saraiki"/>
+    <hyperlink ref="I188" r:id="rId1" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kejom.zip"/>
+    <hyperlink ref="I189" r:id="rId2" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kazakh.zip"/>
+    <hyperlink ref="I190" r:id="rId3" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Jianchuan-bai.ziB"/>
+    <hyperlink ref="I191" r:id="rId4" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kalasha.zip"/>
+    <hyperlink ref="I192" r:id="rId5" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Belarusian.zip"/>
+    <hyperlink ref="I196" r:id="rId6" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Saraiki.zip"/>
+    <hyperlink ref="G198" r:id="rId7" display="https://doi.org/10.1017/S0025100320000201"/>
+    <hyperlink ref="I198" r:id="rId8" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Trapezountian-Greek.zip"/>
+    <hyperlink ref="G199" r:id="rId9" display="https://doi.org/10.1017/S0025100320000225"/>
+    <hyperlink ref="I199" r:id="rId10" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Dagaare.zip"/>
+    <hyperlink ref="G200" r:id="rId11" display="https://doi.org/10.1017/S0025100320000237"/>
+    <hyperlink ref="I200" r:id="rId12" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Ambel.zip"/>
+    <hyperlink ref="G201" r:id="rId13" display="https://doi.org/10.1017/S0025100320000134"/>
+    <hyperlink ref="I201" r:id="rId14" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Arabic-Dialect-Of-Gaza-City.zip"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
recording links for tongan and central lisu
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="815">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -1984,6 +1984,9 @@
     <t xml:space="preserve">https://doi.org/10.1017/S0025100318000129</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Lisu.zip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Philippine English</t>
   </si>
   <si>
@@ -2027,6 +2030,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://doi.org/10.1017/S0025100318000397</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Tongan.zip</t>
   </si>
   <si>
     <t xml:space="preserve">Saterland Frisian</t>
@@ -2666,8 +2672,8 @@
   </sheetPr>
   <dimension ref="A1:J202"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A187" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A202" activeCellId="0" sqref="A202"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E140" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I160" activeCellId="0" sqref="I160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5461,139 +5467,144 @@
       <c r="H160" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="I160" s="0" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="G161" s="0" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="H161" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I161" s="0" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="G162" s="0" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="H162" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I162" s="0" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="H163" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="H164" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I164" s="1"/>
+      <c r="I164" s="1" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="H165" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="H166" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="H167" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="H168" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5601,7 +5612,7 @@
         <v>189</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="G169" s="1" t="s">
         <v>191</v>
@@ -5618,7 +5629,7 @@
         <v>410</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="G170" s="1" t="s">
         <v>412</v>
@@ -5632,546 +5643,546 @@
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="H171" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="H172" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="H173" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="H174" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I174" s="1" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="H175" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I175" s="2" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="H176" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I176" s="2" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="H177" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="H178" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I178" s="1" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="G179" s="0" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="H179" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I179" s="1" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="H180" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I180" s="1" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="H181" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I181" s="0" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="H182" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I182" s="0" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="G183" s="0" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="H183" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I183" s="0" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="H184" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I184" s="1" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="H185" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="H186" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I186" s="0" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="2" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="G187" s="0" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="H187" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I187" s="0" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="G188" s="0" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="H188" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I188" s="4" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="G189" s="0" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="H189" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I189" s="5" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="G190" s="0" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="H190" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I190" s="6" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="2" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="G191" s="0" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="H191" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I191" s="6" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="2" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="G192" s="0" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="H192" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I192" s="6" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="G193" s="0" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="H193" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I193" s="0" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="2" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="G194" s="0" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="H194" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I194" s="0" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="G195" s="0" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="H195" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I195" s="0" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="G196" s="0" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="H196" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I196" s="6" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="G197" s="0" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="H197" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I197" s="0" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="2" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="G198" s="7" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="H198" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I198" s="7" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="2" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="G199" s="7" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="H199" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I199" s="7" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="2" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="G200" s="7" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="H200" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I200" s="7" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="G201" s="7" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="H201" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I201" s="7" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="2" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="G202" s="7" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="H202" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I202" s="7" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cwyzhy Abkhaz, Mojeno Trinitario, Ende
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="827">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -2465,6 +2465,96 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Ladin.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cwyzhy Abkhaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Künceğiz, Turkey </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://doi.org/10.1017/S0025100320000390</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ttps://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Cwyzhy-Abkhaz.zip</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Mojeño Trinitario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trinidad, Bolivia </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://doi.org/10.1017/S0025100320000365</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Mojeno-Trinitario.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malam, Western Province, Papua New Guinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Ende.zip</t>
   </si>
 </sst>
 </file>
@@ -2670,10 +2760,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J202"/>
+  <dimension ref="A1:J205"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E140" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I160" activeCellId="0" sqref="I160"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E171" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I205" activeCellId="0" sqref="I205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6185,6 +6275,57 @@
         <v>814</v>
       </c>
     </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="G203" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="H203" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I203" s="2" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="G204" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="H204" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I204" s="0" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="G205" s="0" t="s">
+        <v>825</v>
+      </c>
+      <c r="H205" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I205" s="0" t="s">
+        <v>826</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I188" r:id="rId1" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Kejom.zip"/>
@@ -6203,6 +6344,9 @@
     <hyperlink ref="I201" r:id="rId14" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Arabic-Dialect-Of-Gaza-City.zip"/>
     <hyperlink ref="G202" r:id="rId15" display="https://doi.org/10.1017/S0025100320000262"/>
     <hyperlink ref="I202" r:id="rId16" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Ladin.zip"/>
+    <hyperlink ref="G203" r:id="rId17" display="https://doi.org/10.1017/S0025100320000390"/>
+    <hyperlink ref="I203" r:id="rId18" display="ttps://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Cwyzhy-Abkhaz.zip"/>
+    <hyperlink ref="G204" r:id="rId19" display="https://doi.org/10.1017/S0025100320000365"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Nafsan, Mecapalapa Tepehua, Northern Tepehuan, Northern Welsh
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="842">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -2471,6 +2471,42 @@
   </si>
   <si>
     <t xml:space="preserve">Künceğiz, Turkey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000390 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Cwyzhy-Abkhaz.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mojeño Trinitario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trinidad, Bolivia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000365 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Mojeno-Trinitario.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malam, Western Province, Papua New Guinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Ende.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nafsan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erakor, Efate, Vanuatu </t>
   </si>
   <si>
     <r>
@@ -2481,7 +2517,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://doi.org/10.1017/S0025100320000390</t>
+      <t xml:space="preserve">https://doi.org/10.1017/S0025100321000177</t>
     </r>
     <r>
       <rPr>
@@ -2494,15 +2530,15 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">h</t>
-    </r>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Nafsan.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mecapalapa Tepehua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mecapalapua, Puebla, Mexico </t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -2511,14 +2547,23 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">ttps://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Cwyzhy-Abkhaz.zip</t>
+      <t xml:space="preserve">https://doi.org/10.1017/S0025100321000098</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Mojeño Trinitario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trinidad, Bolivia </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Tepehuan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sierra Tarahumara, Chihuahua State, Mexico </t>
   </si>
   <si>
     <r>
@@ -2529,7 +2574,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://doi.org/10.1017/S0025100320000365</t>
+      <t xml:space="preserve">https://doi.org/10.1017/S002510032100013X</t>
     </r>
     <r>
       <rPr>
@@ -2538,23 +2583,41 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">  </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Mojeno-Trinitario.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ende</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malam, Western Province, Papua New Guinea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1017/S0025100320000389</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Ende.zip</t>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Northern-Tepehuan.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Welsh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Llŷn Peninsula, Gwynedd County, Wales </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://doi.org/10.1017/S0025100321000165</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Northern-Welsh.zip</t>
   </si>
 </sst>
 </file>
@@ -2564,7 +2627,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2606,6 +2669,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2650,7 +2718,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2680,6 +2748,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2760,10 +2836,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J205"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E171" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I205" activeCellId="0" sqref="I205"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F181" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I209" activeCellId="0" sqref="I209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6288,7 +6364,7 @@
       <c r="H203" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I203" s="2" t="s">
+      <c r="I203" s="7" t="s">
         <v>818</v>
       </c>
     </row>
@@ -6324,6 +6400,75 @@
       </c>
       <c r="I205" s="0" t="s">
         <v>826</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="8" t="s">
+        <v>827</v>
+      </c>
+      <c r="B206" s="9" t="s">
+        <v>828</v>
+      </c>
+      <c r="C206" s="2"/>
+      <c r="G206" s="7" t="s">
+        <v>829</v>
+      </c>
+      <c r="H206" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I206" s="7" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="G207" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="H207" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I207" s="7" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="G208" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="H208" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I208" s="7" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="G209" s="7" t="s">
+        <v>840</v>
+      </c>
+      <c r="H209" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I209" s="7" t="s">
+        <v>841</v>
       </c>
     </row>
   </sheetData>
@@ -6344,9 +6489,17 @@
     <hyperlink ref="I201" r:id="rId14" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Arabic-Dialect-Of-Gaza-City.zip"/>
     <hyperlink ref="G202" r:id="rId15" display="https://doi.org/10.1017/S0025100320000262"/>
     <hyperlink ref="I202" r:id="rId16" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Ladin.zip"/>
-    <hyperlink ref="G203" r:id="rId17" display="https://doi.org/10.1017/S0025100320000390"/>
-    <hyperlink ref="I203" r:id="rId18" display="ttps://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Cwyzhy-Abkhaz.zip"/>
-    <hyperlink ref="G204" r:id="rId19" display="https://doi.org/10.1017/S0025100320000365"/>
+    <hyperlink ref="G203" r:id="rId17" display="https://doi.org/10.1017/S0025100320000390 "/>
+    <hyperlink ref="I203" r:id="rId18" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Cwyzhy-Abkhaz.zip"/>
+    <hyperlink ref="G204" r:id="rId19" display="https://doi.org/10.1017/S0025100320000365 "/>
+    <hyperlink ref="G206" r:id="rId20" display="https://doi.org/10.1017/S0025100321000177"/>
+    <hyperlink ref="I206" r:id="rId21" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Nafsan.zip"/>
+    <hyperlink ref="G207" r:id="rId22" display="https://doi.org/10.1017/S0025100321000098"/>
+    <hyperlink ref="I207" r:id="rId23" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Mojeno-Trinitario.zip"/>
+    <hyperlink ref="G208" r:id="rId24" display="https://doi.org/10.1017/S002510032100013X"/>
+    <hyperlink ref="I208" r:id="rId25" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Northern-Tepehuan.zip"/>
+    <hyperlink ref="G209" r:id="rId26" display="https://doi.org/10.1017/S0025100321000165"/>
+    <hyperlink ref="I209" r:id="rId27" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Northern-Welsh.zip"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Baima, Chukchansi Yokuts, Markina Basque
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="862">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -2570,6 +2570,42 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Qaqet.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pingwu County, Sichuan Province, China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100321000219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Baima.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chukchansi Yokuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Joaquin valley, California, USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100321000268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Chukchansi-Yokuts.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Markina Basque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Markina-Xemein, Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100322000032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Markina-Basque.zip</t>
   </si>
 </sst>
 </file>
@@ -2779,10 +2815,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J211"/>
+  <dimension ref="A1:J214"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F181" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I211" activeCellId="0" sqref="I211"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F184" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I214" activeCellId="0" sqref="I214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6446,6 +6482,57 @@
       </c>
       <c r="I211" s="0" t="s">
         <v>849</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="G212" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="H212" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I212" s="0" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="G213" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="H213" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I213" s="0" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="G214" s="0" t="s">
+        <v>860</v>
+      </c>
+      <c r="H214" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I214" s="0" t="s">
+        <v>861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hefei Mandarin + new analytics
</commit_message>
<xml_diff>
--- a/IPA_Illustrations_enc.xlsx
+++ b/IPA_Illustrations_enc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="866">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -2606,6 +2606,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Markina-Basque.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hefei Mandarin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hefei, Anhui Province, China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1017/S0025100322000081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Hefei-Mandarin.zip</t>
   </si>
 </sst>
 </file>
@@ -2815,10 +2827,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J214"/>
+  <dimension ref="A1:J215"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F184" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I214" activeCellId="0" sqref="I214"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A188" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A215" activeCellId="0" sqref="A215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6533,6 +6545,23 @@
       </c>
       <c r="I214" s="0" t="s">
         <v>861</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="G215" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="H215" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I215" s="7" t="s">
+        <v>865</v>
       </c>
     </row>
   </sheetData>
@@ -6566,6 +6595,8 @@
     <hyperlink ref="I209" r:id="rId27" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Northern-Welsh.zip"/>
     <hyperlink ref="G210" r:id="rId28" display="https://doi.org/10.1017/S0025100321000189 "/>
     <hyperlink ref="I210" r:id="rId29" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Huangyan-Taizhou.zip"/>
+    <hyperlink ref="G215" r:id="rId30" display="https://doi.org/10.1017/S0025100322000081"/>
+    <hyperlink ref="I215" r:id="rId31" display="https://www.internationalphoneticassociation.org/sites/default/files/JIPArecordings/Hefei-Mandarin.zip"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>